<commit_message>
aplicatia e gata. tre sa comentez codu + sa l aranjez + culori
</commit_message>
<xml_diff>
--- a/tasks2.xlsx
+++ b/tasks2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -128,6 +128,39 @@
   </si>
   <si>
     <t>Something Done</t>
+  </si>
+  <si>
+    <t>0|29</t>
+  </si>
+  <si>
+    <t>19%</t>
+  </si>
+  <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>0|31</t>
+  </si>
+  <si>
+    <t>vreau sa fiu cantaret</t>
+  </si>
+  <si>
+    <t>invat notele muzicale</t>
+  </si>
+  <si>
+    <t>50|30</t>
+  </si>
+  <si>
+    <t>sa dansez</t>
+  </si>
+  <si>
+    <t>83|0</t>
+  </si>
+  <si>
+    <t>133|30</t>
+  </si>
+  <si>
+    <t>1%</t>
   </si>
 </sst>
 </file>
@@ -171,11 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="true" applyFill="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -487,7 +523,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD10"/>
@@ -553,7 +589,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
         <v>36</v>
@@ -625,10 +661,10 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7">
@@ -645,10 +681,10 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -668,10 +704,10 @@
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -691,10 +727,10 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -721,6 +757,75 @@
       </c>
       <c r="G10" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" t="n" s="11">
+        <v>48638.52055472222</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="n" s="12">
+        <v>46441.0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="n" s="13">
+        <v>45344.52314275463</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>